<commit_message>
doc: tabela de solicitações
</commit_message>
<xml_diff>
--- a/documentacao/MongoDB/DicionariodeDados.xlsx
+++ b/documentacao/MongoDB/DicionariodeDados.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinic\Documents\SENAI\TCC\documentacao\mongoDocumentacao\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\TCC\documentacao\MongoDB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18DA248A-3BD4-4859-8E2C-C0AD4B14B5C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DCDD5A2-BB91-4C82-A42E-82E2EFA0F0BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="35">
   <si>
     <t>Restrição</t>
   </si>
@@ -106,6 +106,30 @@
   </si>
   <si>
     <t>support</t>
+  </si>
+  <si>
+    <t>solicitation</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> —</t>
+  </si>
+  <si>
+    <t>approved</t>
+  </si>
+  <si>
+    <t>Boolean</t>
+  </si>
+  <si>
+    <t>user_id</t>
+  </si>
+  <si>
+    <t>hospital_id</t>
+  </si>
+  <si>
+    <t>timestamps</t>
+  </si>
+  <si>
+    <t>Date</t>
   </si>
 </sst>
 </file>
@@ -470,10 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="E5:J32"/>
+  <dimension ref="E5:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27:J27"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34:J41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -961,11 +985,162 @@
         <v>21</v>
       </c>
     </row>
+    <row r="34" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E34" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="4"/>
+    </row>
+    <row r="35" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E35" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E36" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J36" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E37" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I37" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J37" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="38" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E38" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I38" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J38" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="39" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E39" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I39" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J39" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="40" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E40" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I40" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J40" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E41" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I41" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J41" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="E5:J5"/>
     <mergeCell ref="E18:J18"/>
     <mergeCell ref="E27:J27"/>
+    <mergeCell ref="E34:J34"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>